<commit_message>
At first he room labeling was hard-coded but I made it label the room based on were your label X on the csv file.
</commit_message>
<xml_diff>
--- a/OurBoardLayout.xlsx
+++ b/OurBoardLayout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MehmetYilmaz/eclipse-workspace/ClueBoard-1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MehmetYilmaz/eclipse-workspace/ClueGame/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="24">
   <si>
     <t>M</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>GR</t>
+  </si>
+  <si>
+    <t>DX</t>
   </si>
 </sst>
 </file>
@@ -398,7 +401,7 @@
   <dimension ref="A1:AF23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R24" sqref="R24"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1776,7 +1779,7 @@
         <v>15</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="M19" s="1" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Added MessageDialog for ClueGame
</commit_message>
<xml_diff>
--- a/OurBoardLayout.xlsx
+++ b/OurBoardLayout.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="23">
   <si>
     <t>M</t>
   </si>
@@ -96,9 +96,6 @@
   </si>
   <si>
     <t>GR</t>
-  </si>
-  <si>
-    <t>DX</t>
   </si>
 </sst>
 </file>
@@ -401,7 +398,7 @@
   <dimension ref="A1:AF23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1779,7 +1776,7 @@
         <v>15</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="M19" s="1" t="s">
         <v>15</v>

</xml_diff>